<commit_message>
actualizacion graficos y tablas
</commit_message>
<xml_diff>
--- a/indicadores/tablas/120101.xlsx
+++ b/indicadores/tablas/120101.xlsx
@@ -504,7 +504,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -814,7 +814,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>